<commit_message>
added scrum board sprint5
</commit_message>
<xml_diff>
--- a/Project_Management/Work_breakdown_structure.xlsx
+++ b/Project_Management/Work_breakdown_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GL704G\Desktop\freecol-SE-exercise\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1FD095-818E-4CFC-AC36-89F420D116C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AFC6C3-43D4-451B-806D-048B11A8558E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{5FF1C84C-74F6-4503-AE0B-EA04810D9109}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{5FF1C84C-74F6-4503-AE0B-EA04810D9109}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -76,11 +76,6 @@
 </t>
   </si>
   <si>
-    <t>1.5.1 - Produce two User Stories for each functionality proposed with a description of   it
-1.5.2 - Apply changes to the code with the respective Unit Tests
-1.5.3 - Create a Demo video of the two functionalaties.</t>
-  </si>
-  <si>
     <t>1.free-col</t>
   </si>
   <si>
@@ -101,6 +96,11 @@
 1.2.2 - Illustrate the code snippet .
 1.2.3 - Provide na explanation of the rationale for identifying the design pattern.
 1.2.4- Provide a class diagram </t>
+  </si>
+  <si>
+    <t>1.5.1 - Produce three User Stories for each functionality proposed with a description of   it
+1.5.2 - Apply changes to the code with the respective Unit Tests when applicable
+1.5.3 - Create a Demo video of the two functionalaties.</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3888A4CC-FC3B-4760-AA58-B4B792B8FF4D}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +542,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -562,13 +562,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -586,19 +586,19 @@
     <row r="7" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>